<commit_message>
RA - letzte Aufgabe (ra-end)
</commit_message>
<xml_diff>
--- a/2/Rechnerarchitektur/Aufgabe 5/Übung 5_2_2 - Vorlage.xlsx
+++ b/2/Rechnerarchitektur/Aufgabe 5/Übung 5_2_2 - Vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mblaich\SynologyDrive\RA_Blaich\SS22\Übungen\05_Aufgabe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombo\HTWG\AIN\2\Rechnerarchitektur\Aufgabe 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C250D967-3DC1-4B3C-82D2-DF86B30CC984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EECD9A1-839E-4599-8D74-FD767B94017A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="20820" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lösung - 5.2.2" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Adresse</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Penalty</t>
-  </si>
-  <si>
-    <t>Penaly</t>
   </si>
   <si>
     <t>Summe</t>
@@ -168,6 +165,27 @@
   </si>
   <si>
     <t>Prozeduren</t>
+  </si>
+  <si>
+    <t>miss</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hit </t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9.75</t>
   </si>
 </sst>
 </file>
@@ -499,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,16 +587,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -608,10 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -623,56 +635,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1020,106 +1031,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFF17A2-FE26-464F-B4D5-8A3B7954C20B}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="58" t="s">
+    <row r="1" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E1" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="60"/>
-    </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="E2" s="45" t="s">
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="47"/>
+    </row>
+    <row r="2" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E2" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="45" t="s">
+      <c r="K2" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="51"/>
-      <c r="N2" s="52"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
+    </row>
+    <row r="3" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E3" s="25"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="52"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="25"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="52"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="61" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="60"/>
+    </row>
+    <row r="4" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="50"/>
-    </row>
-    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="53"/>
+    </row>
+    <row r="5" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -1132,10 +1143,10 @@
         <v>4</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>2</v>
@@ -1147,104 +1158,223 @@
         <v>4</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A6" s="55">
         <v>1</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="11"/>
+      <c r="B6" s="23">
+        <v>2</v>
+      </c>
+      <c r="C6" s="23">
+        <v>250</v>
+      </c>
+      <c r="D6" s="28">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>61</v>
+      </c>
+      <c r="F6" s="24">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="8">
+        <v>125</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0</v>
+      </c>
       <c r="P6" s="18"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A7" s="55"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="10"/>
+      <c r="B7" s="23">
+        <v>3</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2299</v>
+      </c>
+      <c r="D7" s="28">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>60</v>
+      </c>
+      <c r="F7" s="24">
+        <v>5</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="J7" s="8"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="11"/>
+      <c r="O7" s="11">
+        <v>0</v>
+      </c>
       <c r="P7" s="18"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A8" s="55"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="18"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23">
+        <v>5</v>
+      </c>
+      <c r="C8" s="23">
+        <v>760</v>
+      </c>
+      <c r="D8" s="28">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7">
+        <v>61</v>
+      </c>
+      <c r="F8" s="24">
+        <v>17</v>
+      </c>
+      <c r="G8" s="24">
+        <v>4</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="8">
+        <v>125</v>
+      </c>
+      <c r="K8" s="21">
+        <v>8</v>
+      </c>
+      <c r="L8" s="21">
+        <v>4</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A9" s="55">
         <v>2</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="18"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23">
+        <v>250</v>
+      </c>
+      <c r="D9" s="28">
+        <v>4</v>
+      </c>
+      <c r="E9" s="7">
+        <v>61</v>
+      </c>
+      <c r="F9" s="24">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="8">
+        <v>125</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21">
+        <v>4</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="11">
+        <v>2</v>
+      </c>
+      <c r="P9" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A10" s="55"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="10"/>
+      <c r="B10" s="23">
+        <v>3</v>
+      </c>
+      <c r="C10" s="23">
+        <v>2299</v>
+      </c>
+      <c r="D10" s="28">
+        <v>4</v>
+      </c>
+      <c r="E10" s="7">
+        <v>60</v>
+      </c>
+      <c r="F10" s="24">
+        <v>5</v>
+      </c>
+      <c r="G10" s="24">
+        <v>4</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="J10" s="8"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
@@ -1253,16 +1383,32 @@
       <c r="O10" s="11"/>
       <c r="P10" s="18"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A11" s="55"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="10"/>
+      <c r="B11" s="23">
+        <v>5</v>
+      </c>
+      <c r="C11" s="23">
+        <v>761</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>62</v>
+      </c>
+      <c r="F11" s="24">
+        <v>17</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
@@ -1271,91 +1417,186 @@
       <c r="O11" s="11"/>
       <c r="P11" s="18"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A12" s="55">
         <v>3</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="18"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23">
+        <v>2</v>
+      </c>
+      <c r="C12" s="23">
+        <v>251</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>62</v>
+      </c>
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="8">
+        <v>126</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="21">
+        <v>0</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="11">
+        <v>2</v>
+      </c>
+      <c r="P12" s="18">
+        <v>10</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A13" s="55"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="9"/>
+      <c r="B13" s="23">
+        <v>3</v>
+      </c>
+      <c r="C13" s="23">
+        <v>2300</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>61</v>
+      </c>
+      <c r="F13" s="24">
+        <v>5</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="8">
+        <v>125</v>
+      </c>
+      <c r="K13" s="21">
+        <v>2</v>
+      </c>
+      <c r="L13" s="21">
+        <v>0</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="O13" s="11"/>
       <c r="P13" s="18"/>
     </row>
-    <row r="14" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="56"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="41"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="27">
+        <v>5</v>
+      </c>
+      <c r="C14" s="27">
+        <v>761</v>
+      </c>
+      <c r="D14" s="29">
+        <v>4</v>
+      </c>
+      <c r="E14" s="31">
+        <v>62</v>
+      </c>
+      <c r="F14" s="32">
+        <v>17</v>
+      </c>
+      <c r="G14" s="32">
+        <v>4</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="35">
+        <v>126</v>
+      </c>
+      <c r="K14" s="36">
+        <v>8</v>
+      </c>
+      <c r="L14" s="36">
+        <v>4</v>
+      </c>
+      <c r="M14" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="39"/>
+      <c r="P14" s="40"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.5">
       <c r="F15" s="22"/>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="J15" s="42"/>
-      <c r="L15" s="31" t="s">
+      <c r="H15" s="30">
+        <v>6</v>
+      </c>
+      <c r="J15" s="22"/>
+      <c r="L15" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="31"/>
-      <c r="O15" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="39"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M15" s="30">
+        <v>2</v>
+      </c>
+      <c r="O15" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.5">
       <c r="F16" s="22"/>
       <c r="G16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="1">
+        <v>60</v>
+      </c>
+      <c r="J16" s="22"/>
       <c r="L16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="M16" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
@@ -1363,14 +1604,14 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A18" s="57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="57"/>
       <c r="C18" s="57"/>
       <c r="D18" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -1378,94 +1619,100 @@
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="5"/>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A19" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="5">
+        <v>32</v>
+      </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="5"/>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A20" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="5">
+        <v>60</v>
+      </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="5">
+        <v>200</v>
+      </c>
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="5">
+        <v>20</v>
+      </c>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="5"/>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A23" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="5">
+        <v>312</v>
+      </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A24" s="54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="54"/>
       <c r="C24" s="54"/>
-      <c r="D24" s="47"/>
+      <c r="D24" s="61" t="s">
+        <v>51</v>
+      </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L30" s="48"/>
-    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="M2:N3"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -1473,12 +1720,11 @@
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="H2:I3"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="M2:N3"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="E4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1490,128 +1736,128 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>